<commit_message>
Feedback related to mumbai district and ela
</commit_message>
<xml_diff>
--- a/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12241 Vitamin A1 Performance/38. Vitamin A1 performance report.xlsx
+++ b/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12241 Vitamin A1 Performance/38. Vitamin A1 performance report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="23895" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t>State Family Welfare Bureau,Pune</t>
   </si>
@@ -113,9 +113,15 @@
     <t>J-O</t>
   </si>
   <si>
+    <t>Rural Group</t>
+  </si>
+  <si>
     <t>1. Use following groups for District Total fields:</t>
   </si>
   <si>
+    <t>Corporation Group</t>
+  </si>
+  <si>
     <t>DH - Rural</t>
   </si>
   <si>
@@ -162,9 +168,6 @@
   </si>
   <si>
     <t>UDH Group</t>
-  </si>
-  <si>
-    <t>Corporation Group</t>
   </si>
 </sst>
 </file>
@@ -172,12 +175,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +211,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9.75"/>
+      <color rgb="FF263238"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -218,6 +227,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9.75"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Verdana"/>
@@ -231,9 +246,69 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,46 +322,61 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,81 +389,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -396,13 +411,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,37 +513,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,127 +579,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -666,17 +681,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,6 +729,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -719,201 +778,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -949,18 +964,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1285,7 +1306,7 @@
   <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1339,7 +1360,7 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="16"/>
+      <c r="P2" s="18"/>
     </row>
     <row r="3" ht="17.25" spans="1:16">
       <c r="A3" s="5" t="s">
@@ -1374,7 +1395,7 @@
       <c r="N3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="17" t="s">
+      <c r="O3" s="19" t="s">
         <v>11</v>
       </c>
       <c r="P3" s="5" t="s">
@@ -1452,107 +1473,113 @@
       <c r="L5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="18" t="s">
+      <c r="M5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="18" t="s">
+      <c r="N5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="18" t="s">
+      <c r="O5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" ht="22.5" spans="6:6">
-      <c r="F7" s="14" t="s">
+    <row r="7" ht="22.5" spans="3:6">
+      <c r="C7" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="6:6">
-      <c r="F8" s="15" t="s">
+      <c r="F7" s="15" t="s">
         <v>33</v>
       </c>
     </row>
+    <row r="8" spans="3:6">
+      <c r="C8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="9" spans="6:6">
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="6:6">
+      <c r="F10" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="6:6">
+      <c r="F11" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="6:6">
+      <c r="F12" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="6:6">
+      <c r="F13" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="6:6">
+      <c r="F14" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="6:6">
+      <c r="F15" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="6:6">
+      <c r="F16" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6">
+      <c r="F17" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6">
+      <c r="F18" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" ht="22.5" spans="6:6">
+      <c r="F20" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6">
+      <c r="F21" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6">
+      <c r="F22" s="17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6">
+      <c r="F23" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6">
+      <c r="F24" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6">
+      <c r="F25" s="17" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="6:6">
-      <c r="F10" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="6:6">
-      <c r="F11" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="6:6">
-      <c r="F12" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="6:6">
-      <c r="F13" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="6:6">
-      <c r="F14" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="6:6">
-      <c r="F15" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="6:6">
-      <c r="F16" s="15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6">
-      <c r="F17" s="15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6">
-      <c r="F18" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" ht="22.5" spans="6:6">
-      <c r="F20" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="6:6">
-      <c r="F21" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="6:6">
-      <c r="F22" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="6:6">
-      <c r="F23" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="6:6">
-      <c r="F24" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="6:6">
-      <c r="F25" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vitamin A1 report updated
</commit_message>
<xml_diff>
--- a/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12241 Vitamin A1 Performance/38. Vitamin A1 performance report.xlsx
+++ b/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12241 Vitamin A1 Performance/38. Vitamin A1 performance report.xlsx
@@ -97,7 +97,7 @@
     <t>(J/C)*100</t>
   </si>
   <si>
-    <t>(J/D)*100</t>
+    <t>(I/D)*100</t>
   </si>
   <si>
     <t>When L is &lt;60%, then 0
@@ -175,10 +175,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -247,6 +247,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -254,14 +261,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -277,19 +284,43 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -298,9 +329,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,7 +353,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,71 +367,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -411,187 +411,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,6 +685,60 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -701,30 +755,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -748,183 +778,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1305,8 +1305,8 @@
   <sheetPr/>
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>